<commit_message>
music artt add artrt—_score, eduadmin aladmin finish
</commit_message>
<xml_diff>
--- a/批量导入模板/音乐教师模板/期末音乐教师考核模板.xlsx
+++ b/批量导入模板/音乐教师模板/期末音乐教师考核模板.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myGithub\ynyzjs\teacher_system\批量导入模板\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myGithub\ynyzjs\teacher_system\批量导入模板\音乐教师模板\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAD72BD-E03D-450F-8A2E-F933F800F955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84C13A2-5733-4942-910D-C11E8A0C45A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>学期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,6 +125,10 @@
   </si>
   <si>
     <t>2025.2.19-7.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下学期艺考赋分</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -472,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -492,11 +496,12 @@
     <col min="11" max="11" width="14.375" style="1" customWidth="1"/>
     <col min="12" max="12" width="15.625" style="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="1"/>
+    <col min="14" max="14" width="14" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,13 +542,16 @@
         <v>24</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -584,10 +592,13 @@
         <v>1</v>
       </c>
       <c r="N2" s="1">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -628,10 +639,13 @@
         <v>1</v>
       </c>
       <c r="N3" s="1">
+        <v>9</v>
+      </c>
+      <c r="O3" s="1">
         <v>2.9849999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -672,10 +686,13 @@
         <v>1</v>
       </c>
       <c r="N4" s="1">
+        <v>9</v>
+      </c>
+      <c r="O4" s="1">
         <v>2.9699999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -716,10 +733,13 @@
         <v>1</v>
       </c>
       <c r="N5" s="1">
+        <v>9</v>
+      </c>
+      <c r="O5" s="1">
         <v>2.9699999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -760,10 +780,13 @@
         <v>1</v>
       </c>
       <c r="N6" s="1">
+        <v>9</v>
+      </c>
+      <c r="O6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -804,10 +827,13 @@
         <v>1</v>
       </c>
       <c r="N7" s="1">
+        <v>9</v>
+      </c>
+      <c r="O7" s="1">
         <v>2.9699999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -848,10 +874,13 @@
         <v>1</v>
       </c>
       <c r="N8" s="1">
+        <v>9</v>
+      </c>
+      <c r="O8" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -892,6 +921,9 @@
         <v>0.98</v>
       </c>
       <c r="N9" s="1">
+        <v>9</v>
+      </c>
+      <c r="O9" s="1">
         <v>2.9550000000000001</v>
       </c>
     </row>

</xml_diff>